<commit_message>
Filled Leetcode Sheet till 20
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\Contest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252993F7-5F80-4D02-B120-569F77889808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD466BB-8040-4139-B263-D738C7A0B3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6717" uniqueCount="3366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6697" uniqueCount="3366">
   <si>
     <t>ID</t>
   </si>
@@ -10548,8 +10548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1636" workbookViewId="0">
-      <selection activeCell="D1654" sqref="D1654"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="I150" sqref="I150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12673,8 +12673,8 @@
       <c r="C151" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E151" s="9" t="s">
-        <v>8</v>
+      <c r="E151" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12841,8 +12841,8 @@
       <c r="C163" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E163" s="9" t="s">
-        <v>8</v>
+      <c r="E163" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12855,8 +12855,8 @@
       <c r="C164" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E164" s="9" t="s">
-        <v>8</v>
+      <c r="E164" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12869,8 +12869,8 @@
       <c r="C165" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E165" s="9" t="s">
-        <v>8</v>
+      <c r="E165" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -18287,8 +18287,8 @@
       <c r="C552" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E552" s="9" t="s">
-        <v>8</v>
+      <c r="E552" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="553" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -19561,8 +19561,8 @@
       <c r="C643" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E643" s="9" t="s">
-        <v>8</v>
+      <c r="E643" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="644" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -27219,8 +27219,8 @@
       <c r="C1190" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1190" s="9" t="s">
-        <v>8</v>
+      <c r="E1190" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1191" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -28899,8 +28899,8 @@
       <c r="C1310" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1310" s="9" t="s">
-        <v>8</v>
+      <c r="E1310" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1311" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -29809,8 +29809,8 @@
       <c r="C1375" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1375" s="9" t="s">
-        <v>8</v>
+      <c r="E1375" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1376" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -30299,8 +30299,8 @@
       <c r="C1410" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1410" s="9" t="s">
-        <v>8</v>
+      <c r="E1410" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1411" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -31531,8 +31531,8 @@
       <c r="C1498" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1498" s="9" t="s">
-        <v>8</v>
+      <c r="E1498" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1499" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -31587,8 +31587,8 @@
       <c r="C1502" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1502" s="9" t="s">
-        <v>8</v>
+      <c r="E1502" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1503" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32357,8 +32357,8 @@
       <c r="C1557" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1557" s="9" t="s">
-        <v>8</v>
+      <c r="E1557" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1558" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32371,8 +32371,8 @@
       <c r="C1558" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1558" s="9" t="s">
-        <v>8</v>
+      <c r="E1558" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1559" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32385,8 +32385,8 @@
       <c r="C1559" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1559" s="9" t="s">
-        <v>8</v>
+      <c r="E1559" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1560" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33029,8 +33029,8 @@
       <c r="C1605" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1605" s="9" t="s">
-        <v>8</v>
+      <c r="E1605" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1606" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33071,8 +33071,8 @@
       <c r="C1608" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1608" s="9" t="s">
-        <v>8</v>
+      <c r="E1608" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1609" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33309,8 +33309,8 @@
       <c r="C1625" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1625" s="9" t="s">
-        <v>8</v>
+      <c r="E1625" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1626" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33337,8 +33337,8 @@
       <c r="C1627" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1627" s="9" t="s">
-        <v>8</v>
+      <c r="E1627" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1628" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33449,8 +33449,8 @@
       <c r="C1635" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1635" s="9" t="s">
-        <v>8</v>
+      <c r="E1635" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1636" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -35755,5 +35755,6 @@
     <hyperlink ref="D1649" r:id="rId1679" xr:uid="{6783BC4D-2322-4ECC-B313-3BFDFD03DD43}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1680"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Marked till 70 Leetcode Full Sheet
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD466BB-8040-4139-B263-D738C7A0B3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE4ED80-18D8-4C15-9EA9-B0E807DF47B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6697" uniqueCount="3366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3366">
   <si>
     <t>ID</t>
   </si>
@@ -10548,8 +10548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="I150" sqref="I150"/>
+    <sheetView tabSelected="1" topLeftCell="A1271" workbookViewId="0">
+      <selection activeCell="E1284" sqref="E1284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12043,8 +12043,8 @@
       <c r="C106" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E106" s="9" t="s">
-        <v>8</v>
+      <c r="E106" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12281,8 +12281,8 @@
       <c r="C123" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E123" s="9" t="s">
-        <v>8</v>
+      <c r="E123" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12533,8 +12533,8 @@
       <c r="C141" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E141" s="9" t="s">
-        <v>8</v>
+      <c r="E141" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12547,8 +12547,8 @@
       <c r="C142" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E142" s="9" t="s">
-        <v>8</v>
+      <c r="E142" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12589,8 +12589,8 @@
       <c r="C145" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E145" s="9" t="s">
-        <v>8</v>
+      <c r="E145" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12603,8 +12603,8 @@
       <c r="C146" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E146" s="9" t="s">
-        <v>8</v>
+      <c r="E146" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12659,8 +12659,8 @@
       <c r="C150" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E150" s="9" t="s">
-        <v>8</v>
+      <c r="E150" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12729,8 +12729,8 @@
       <c r="C155" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E155" s="9" t="s">
-        <v>8</v>
+      <c r="E155" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -12743,8 +12743,8 @@
       <c r="C156" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E156" s="9" t="s">
-        <v>8</v>
+      <c r="E156" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -14955,8 +14955,8 @@
       <c r="C314" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E314" s="9" t="s">
-        <v>8</v>
+      <c r="E314" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -16565,8 +16565,8 @@
       <c r="C429" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E429" s="9" t="s">
-        <v>8</v>
+      <c r="E429" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -20541,8 +20541,8 @@
       <c r="C713" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E713" s="9" t="s">
-        <v>8</v>
+      <c r="E713" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="714" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -21045,8 +21045,8 @@
       <c r="C749" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E749" s="9" t="s">
-        <v>8</v>
+      <c r="E749" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="750" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -21563,8 +21563,8 @@
       <c r="C786" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E786" s="9" t="s">
-        <v>8</v>
+      <c r="E786" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="787" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -21997,8 +21997,8 @@
       <c r="C817" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E817" s="9" t="s">
-        <v>8</v>
+      <c r="E817" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="818" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -22179,8 +22179,8 @@
       <c r="C830" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E830" s="9" t="s">
-        <v>8</v>
+      <c r="E830" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="831" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -22417,8 +22417,8 @@
       <c r="C847" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E847" s="9" t="s">
-        <v>8</v>
+      <c r="E847" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="848" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -22529,8 +22529,8 @@
       <c r="C855" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E855" s="9" t="s">
-        <v>8</v>
+      <c r="E855" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="856" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -22697,8 +22697,8 @@
       <c r="C867" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E867" s="9" t="s">
-        <v>8</v>
+      <c r="E867" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="868" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -24181,8 +24181,8 @@
       <c r="C973" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E973" s="9" t="s">
-        <v>8</v>
+      <c r="E973" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="974" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -24573,8 +24573,8 @@
       <c r="C1001" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1001" s="9" t="s">
-        <v>8</v>
+      <c r="E1001" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1002" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -25623,8 +25623,8 @@
       <c r="C1076" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1076" s="9" t="s">
-        <v>8</v>
+      <c r="E1076" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1077" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -26323,8 +26323,8 @@
       <c r="C1126" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1126" s="9" t="s">
-        <v>8</v>
+      <c r="E1126" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1127" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -27471,8 +27471,8 @@
       <c r="C1208" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1208" s="9" t="s">
-        <v>8</v>
+      <c r="E1208" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1209" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -27513,8 +27513,8 @@
       <c r="C1211" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1211" s="9" t="s">
-        <v>8</v>
+      <c r="E1211" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1212" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -28045,8 +28045,8 @@
       <c r="C1249" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1249" s="9" t="s">
-        <v>8</v>
+      <c r="E1249" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1250" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -28493,8 +28493,8 @@
       <c r="C1281" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1281" s="9" t="s">
-        <v>8</v>
+      <c r="E1281" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1282" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -28535,8 +28535,8 @@
       <c r="C1284" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1284" s="9" t="s">
-        <v>8</v>
+      <c r="E1284" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1285" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -28969,8 +28969,8 @@
       <c r="C1315" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1315" s="9" t="s">
-        <v>8</v>
+      <c r="E1315" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1316" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -29151,8 +29151,8 @@
       <c r="C1328" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1328" s="9" t="s">
-        <v>8</v>
+      <c r="E1328" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1329" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -29641,8 +29641,8 @@
       <c r="C1363" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1363" s="9" t="s">
-        <v>8</v>
+      <c r="E1363" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1364" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -29949,8 +29949,8 @@
       <c r="C1385" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1385" s="9" t="s">
-        <v>8</v>
+      <c r="E1385" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1386" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -30901,8 +30901,8 @@
       <c r="C1453" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1453" s="9" t="s">
-        <v>8</v>
+      <c r="E1453" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1454" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -31419,8 +31419,8 @@
       <c r="C1490" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1490" s="9" t="s">
-        <v>8</v>
+      <c r="E1490" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1491" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -31545,8 +31545,8 @@
       <c r="C1499" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1499" s="9" t="s">
-        <v>8</v>
+      <c r="E1499" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1500" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -31657,8 +31657,8 @@
       <c r="C1507" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1507" s="9" t="s">
-        <v>8</v>
+      <c r="E1507" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1508" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32105,8 +32105,8 @@
       <c r="C1539" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1539" s="9" t="s">
-        <v>8</v>
+      <c r="E1539" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1540" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32245,8 +32245,8 @@
       <c r="C1549" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1549" s="9" t="s">
-        <v>8</v>
+      <c r="E1549" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1550" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32441,8 +32441,8 @@
       <c r="C1563" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1563" s="9" t="s">
-        <v>8</v>
+      <c r="E1563" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1564" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32623,8 +32623,8 @@
       <c r="C1576" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1576" s="9" t="s">
-        <v>8</v>
+      <c r="E1576" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1577" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32707,8 +32707,8 @@
       <c r="C1582" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1582" s="9" t="s">
-        <v>8</v>
+      <c r="E1582" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1583" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32763,8 +32763,8 @@
       <c r="C1586" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1586" s="9" t="s">
-        <v>8</v>
+      <c r="E1586" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1587" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -32959,8 +32959,8 @@
       <c r="C1600" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1600" s="9" t="s">
-        <v>8</v>
+      <c r="E1600" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1601" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33225,8 +33225,8 @@
       <c r="C1619" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1619" s="9" t="s">
-        <v>8</v>
+      <c r="E1619" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1620" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33253,8 +33253,8 @@
       <c r="C1621" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1621" s="9" t="s">
-        <v>8</v>
+      <c r="E1621" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1622" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33519,8 +33519,8 @@
       <c r="C1640" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1640" s="9" t="s">
-        <v>8</v>
+      <c r="E1640" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1641" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33533,8 +33533,8 @@
       <c r="C1641" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1641" s="9" t="s">
-        <v>8</v>
+      <c r="E1641" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1642" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -33746,8 +33746,8 @@
       <c r="C1656" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1656" s="9" t="s">
-        <v>8</v>
+      <c r="E1656" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1657" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -34068,8 +34068,8 @@
       <c r="C1679" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1679" s="9" t="s">
-        <v>8</v>
+      <c r="E1679" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Search in Rotated Sorted Array
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA4053-E25F-4759-A2EF-3A0BE341BF2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C68B98E-2070-4B1C-846F-09AFFFB3337C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6609" uniqueCount="3368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6609" uniqueCount="3369">
   <si>
     <t>ID</t>
   </si>
@@ -10135,6 +10135,9 @@
   </si>
   <si>
     <t>Clue: At each position, check for each cell which one gives the best answer to reach current cell</t>
+  </si>
+  <si>
+    <t>Explanation in java file itself</t>
   </si>
 </sst>
 </file>
@@ -10557,8 +10560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11047,8 +11050,11 @@
       <c r="C34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>8</v>
+      <c r="D34" t="s">
+        <v>3368</v>
+      </c>
+      <c r="E34" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Daily Challenge 7/5/2021
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB8965F-C9E5-450B-B0AE-EB1B0E350409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63BB9ED-AD66-41EC-BFAC-4CE0AD7F39F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6606" uniqueCount="3371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="3371">
   <si>
     <t>ID</t>
   </si>
@@ -10566,8 +10566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A946" workbookViewId="0">
-      <selection activeCell="I955" sqref="I955"/>
+    <sheetView tabSelected="1" topLeftCell="A526" workbookViewId="0">
+      <selection activeCell="D541" sqref="D541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18205,8 +18205,8 @@
       <c r="C544" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E544" s="8" t="s">
-        <v>8</v>
+      <c r="E544" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="545" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Another Binary Search Question
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63BB9ED-AD66-41EC-BFAC-4CE0AD7F39F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B36852D-5925-4138-8D0D-4244F97E940C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="3371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="3372">
   <si>
     <t>ID</t>
   </si>
@@ -10144,6 +10144,9 @@
   </si>
   <si>
     <t>Explanation in Solution File</t>
+  </si>
+  <si>
+    <t>Full Explanation in Code File</t>
   </si>
 </sst>
 </file>
@@ -10566,8 +10569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A526" workbookViewId="0">
-      <selection activeCell="D541" sqref="D541"/>
+    <sheetView tabSelected="1" topLeftCell="A957" workbookViewId="0">
+      <selection activeCell="H971" sqref="H971"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -24161,8 +24164,11 @@
       <c r="C969" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E969" s="8" t="s">
-        <v>8</v>
+      <c r="D969" t="s">
+        <v>3371</v>
+      </c>
+      <c r="E969" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="970" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Another bianry search probelm: Koko Eating Bananas
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B36852D-5925-4138-8D0D-4244F97E940C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79515B1-2697-4715-A0B2-15DAA7C0691C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10569,8 +10569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A957" workbookViewId="0">
-      <selection activeCell="H971" sqref="H971"/>
+    <sheetView tabSelected="1" topLeftCell="A813" workbookViewId="0">
+      <selection activeCell="E825" sqref="E825"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -22145,8 +22145,11 @@
       <c r="C825" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E825" s="8" t="s">
-        <v>8</v>
+      <c r="D825" t="s">
+        <v>3371</v>
+      </c>
+      <c r="E825" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="826" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 2 problems in Weekly Contest 240
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79515B1-2697-4715-A0B2-15DAA7C0691C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B15A64-E7DA-4A48-B8D1-612B4360C1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$E$1:$E$1679</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$E$1:$E$1683</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="3372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6618" uniqueCount="3379">
   <si>
     <t>ID</t>
   </si>
@@ -10147,6 +10147,27 @@
   </si>
   <si>
     <t>Full Explanation in Code File</t>
+  </si>
+  <si>
+    <t>Maximum Population Year</t>
+  </si>
+  <si>
+    <t>1855</t>
+  </si>
+  <si>
+    <t>Maximum Distance Between a Pair of Values</t>
+  </si>
+  <si>
+    <t>1856</t>
+  </si>
+  <si>
+    <t>1857</t>
+  </si>
+  <si>
+    <t>Largest Color Value in a Directed Graph</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Min-Product</t>
   </si>
 </sst>
 </file>
@@ -10237,7 +10258,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10263,6 +10284,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -10567,10 +10589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1679"/>
+  <dimension ref="A1:E1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A813" workbookViewId="0">
-      <selection activeCell="E825" sqref="E825"/>
+    <sheetView tabSelected="1" topLeftCell="A1580" workbookViewId="0">
+      <selection activeCell="J1580" sqref="J1580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32743,39 +32765,39 @@
       </c>
     </row>
     <row r="1582" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1582" s="10" t="s">
-        <v>203</v>
+      <c r="A1582" s="11">
+        <v>1854</v>
       </c>
       <c r="B1582" s="1" t="s">
-        <v>204</v>
+        <v>3372</v>
       </c>
       <c r="C1582" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1582" s="8" t="s">
-        <v>8</v>
+      <c r="E1582" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1583" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1583" s="10" t="s">
-        <v>201</v>
+      <c r="A1583" s="11" t="s">
+        <v>3373</v>
       </c>
       <c r="B1583" s="1" t="s">
-        <v>202</v>
+        <v>3374</v>
       </c>
       <c r="C1583" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1583" s="8" t="s">
-        <v>8</v>
+      <c r="E1583" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1584" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1584" s="10" t="s">
-        <v>199</v>
+      <c r="A1584" s="11" t="s">
+        <v>3375</v>
       </c>
       <c r="B1584" s="1" t="s">
-        <v>200</v>
+        <v>3378</v>
       </c>
       <c r="C1584" s="5" t="s">
         <v>11</v>
@@ -32785,11 +32807,11 @@
       </c>
     </row>
     <row r="1585" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1585" s="10" t="s">
-        <v>197</v>
+      <c r="A1585" s="11" t="s">
+        <v>3376</v>
       </c>
       <c r="B1585" s="1" t="s">
-        <v>198</v>
+        <v>3377</v>
       </c>
       <c r="C1585" s="4" t="s">
         <v>7</v>
@@ -32800,13 +32822,13 @@
     </row>
     <row r="1586" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1586" s="10" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B1586" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C1586" s="4" t="s">
-        <v>7</v>
+        <v>204</v>
+      </c>
+      <c r="C1586" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1586" s="8" t="s">
         <v>8</v>
@@ -32814,10 +32836,10 @@
     </row>
     <row r="1587" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1587" s="10" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B1587" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C1587" s="5" t="s">
         <v>11</v>
@@ -32828,13 +32850,13 @@
     </row>
     <row r="1588" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1588" s="10" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B1588" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1588" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
+      </c>
+      <c r="C1588" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1588" s="8" t="s">
         <v>8</v>
@@ -32842,13 +32864,13 @@
     </row>
     <row r="1589" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1589" s="10" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B1589" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1589" s="5" t="s">
-        <v>11</v>
+        <v>198</v>
+      </c>
+      <c r="C1589" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1589" s="8" t="s">
         <v>8</v>
@@ -32856,13 +32878,13 @@
     </row>
     <row r="1590" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1590" s="10" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B1590" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1590" s="6" t="s">
-        <v>14</v>
+        <v>196</v>
+      </c>
+      <c r="C1590" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1590" s="8" t="s">
         <v>8</v>
@@ -32870,10 +32892,10 @@
     </row>
     <row r="1591" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1591" s="10" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B1591" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C1591" s="5" t="s">
         <v>11</v>
@@ -32884,10 +32906,10 @@
     </row>
     <row r="1592" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1592" s="10" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B1592" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C1592" s="4" t="s">
         <v>7</v>
@@ -32898,10 +32920,10 @@
     </row>
     <row r="1593" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1593" s="10" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B1593" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C1593" s="5" t="s">
         <v>11</v>
@@ -32912,10 +32934,10 @@
     </row>
     <row r="1594" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1594" s="10" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B1594" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C1594" s="6" t="s">
         <v>14</v>
@@ -32926,10 +32948,10 @@
     </row>
     <row r="1595" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1595" s="10" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B1595" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C1595" s="5" t="s">
         <v>11</v>
@@ -32940,13 +32962,13 @@
     </row>
     <row r="1596" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1596" s="10" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B1596" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1596" s="5" t="s">
-        <v>11</v>
+        <v>184</v>
+      </c>
+      <c r="C1596" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1596" s="8" t="s">
         <v>8</v>
@@ -32954,13 +32976,13 @@
     </row>
     <row r="1597" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1597" s="10" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B1597" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C1597" s="4" t="s">
-        <v>7</v>
+        <v>182</v>
+      </c>
+      <c r="C1597" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1597" s="8" t="s">
         <v>8</v>
@@ -32968,13 +32990,13 @@
     </row>
     <row r="1598" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1598" s="10" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1598" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1598" s="5" t="s">
-        <v>11</v>
+        <v>180</v>
+      </c>
+      <c r="C1598" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1598" s="8" t="s">
         <v>8</v>
@@ -32982,13 +33004,13 @@
     </row>
     <row r="1599" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1599" s="10" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B1599" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1599" s="6" t="s">
-        <v>14</v>
+        <v>178</v>
+      </c>
+      <c r="C1599" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1599" s="8" t="s">
         <v>8</v>
@@ -32996,10 +33018,10 @@
     </row>
     <row r="1600" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1600" s="10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B1600" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C1600" s="5" t="s">
         <v>11</v>
@@ -33010,13 +33032,13 @@
     </row>
     <row r="1601" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1601" s="10" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B1601" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1601" s="5" t="s">
-        <v>11</v>
+        <v>174</v>
+      </c>
+      <c r="C1601" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1601" s="8" t="s">
         <v>8</v>
@@ -33024,13 +33046,13 @@
     </row>
     <row r="1602" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1602" s="10" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B1602" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1602" s="4" t="s">
-        <v>7</v>
+        <v>172</v>
+      </c>
+      <c r="C1602" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1602" s="8" t="s">
         <v>8</v>
@@ -33038,10 +33060,10 @@
     </row>
     <row r="1603" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1603" s="10" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B1603" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C1603" s="6" t="s">
         <v>14</v>
@@ -33052,10 +33074,10 @@
     </row>
     <row r="1604" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1604" s="10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B1604" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C1604" s="5" t="s">
         <v>11</v>
@@ -33066,10 +33088,10 @@
     </row>
     <row r="1605" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1605" s="10" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B1605" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C1605" s="5" t="s">
         <v>11</v>
@@ -33080,10 +33102,10 @@
     </row>
     <row r="1606" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1606" s="10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B1606" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C1606" s="4" t="s">
         <v>7</v>
@@ -33094,13 +33116,13 @@
     </row>
     <row r="1607" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1607" s="10" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B1607" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1607" s="5" t="s">
-        <v>11</v>
+        <v>162</v>
+      </c>
+      <c r="C1607" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1607" s="8" t="s">
         <v>8</v>
@@ -33108,13 +33130,13 @@
     </row>
     <row r="1608" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1608" s="10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B1608" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1608" s="6" t="s">
-        <v>14</v>
+        <v>160</v>
+      </c>
+      <c r="C1608" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1608" s="8" t="s">
         <v>8</v>
@@ -33122,10 +33144,10 @@
     </row>
     <row r="1609" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1609" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B1609" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C1609" s="5" t="s">
         <v>11</v>
@@ -33136,13 +33158,13 @@
     </row>
     <row r="1610" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1610" s="10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B1610" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1610" s="5" t="s">
-        <v>11</v>
+        <v>156</v>
+      </c>
+      <c r="C1610" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1610" s="8" t="s">
         <v>8</v>
@@ -33150,13 +33172,13 @@
     </row>
     <row r="1611" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1611" s="10" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B1611" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1611" s="4" t="s">
-        <v>7</v>
+        <v>154</v>
+      </c>
+      <c r="C1611" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1611" s="8" t="s">
         <v>8</v>
@@ -33164,10 +33186,10 @@
     </row>
     <row r="1612" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1612" s="10" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B1612" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C1612" s="6" t="s">
         <v>14</v>
@@ -33178,10 +33200,10 @@
     </row>
     <row r="1613" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1613" s="10" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B1613" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C1613" s="5" t="s">
         <v>11</v>
@@ -33192,10 +33214,10 @@
     </row>
     <row r="1614" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1614" s="10" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B1614" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C1614" s="5" t="s">
         <v>11</v>
@@ -33206,10 +33228,10 @@
     </row>
     <row r="1615" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1615" s="10" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B1615" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C1615" s="4" t="s">
         <v>7</v>
@@ -33220,13 +33242,13 @@
     </row>
     <row r="1616" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1616" s="10" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B1616" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1616" s="5" t="s">
-        <v>11</v>
+        <v>144</v>
+      </c>
+      <c r="C1616" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1616" s="8" t="s">
         <v>8</v>
@@ -33234,38 +33256,38 @@
     </row>
     <row r="1617" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1617" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B1617" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1617" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1617" s="9" t="b">
-        <v>1</v>
+        <v>142</v>
+      </c>
+      <c r="C1617" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1617" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1618" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1618" s="10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B1618" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C1618" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1618" s="9" t="b">
-        <v>1</v>
+      <c r="E1618" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1619" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1619" s="10" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B1619" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C1619" s="4" t="s">
         <v>7</v>
@@ -33276,13 +33298,13 @@
     </row>
     <row r="1620" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1620" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B1620" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1620" s="4" t="s">
-        <v>7</v>
+        <v>136</v>
+      </c>
+      <c r="C1620" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1620" s="8" t="s">
         <v>8</v>
@@ -33290,41 +33312,41 @@
     </row>
     <row r="1621" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1621" s="10" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B1621" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1621" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1621" s="8" t="s">
-        <v>8</v>
+        <v>134</v>
+      </c>
+      <c r="C1621" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1621" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1622" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1622" s="10" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B1622" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1622" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1622" s="8" t="s">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="C1622" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1622" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1623" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1623" s="10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B1623" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1623" s="5" t="s">
-        <v>11</v>
+        <v>130</v>
+      </c>
+      <c r="C1623" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1623" s="8" t="s">
         <v>8</v>
@@ -33332,13 +33354,13 @@
     </row>
     <row r="1624" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1624" s="10" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B1624" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1624" s="5" t="s">
-        <v>11</v>
+        <v>128</v>
+      </c>
+      <c r="C1624" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1624" s="8" t="s">
         <v>8</v>
@@ -33346,13 +33368,13 @@
     </row>
     <row r="1625" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1625" s="10" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B1625" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1625" s="4" t="s">
-        <v>7</v>
+        <v>126</v>
+      </c>
+      <c r="C1625" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1625" s="8" t="s">
         <v>8</v>
@@ -33360,10 +33382,10 @@
     </row>
     <row r="1626" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1626" s="10" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B1626" s="1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C1626" s="6" t="s">
         <v>14</v>
@@ -33374,10 +33396,10 @@
     </row>
     <row r="1627" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1627" s="10" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B1627" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C1627" s="5" t="s">
         <v>11</v>
@@ -33388,10 +33410,10 @@
     </row>
     <row r="1628" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1628" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B1628" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C1628" s="5" t="s">
         <v>11</v>
@@ -33402,10 +33424,10 @@
     </row>
     <row r="1629" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1629" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B1629" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C1629" s="4" t="s">
         <v>7</v>
@@ -33416,13 +33438,13 @@
     </row>
     <row r="1630" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1630" s="10" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B1630" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1630" s="5" t="s">
-        <v>11</v>
+        <v>116</v>
+      </c>
+      <c r="C1630" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1630" s="8" t="s">
         <v>8</v>
@@ -33430,13 +33452,13 @@
     </row>
     <row r="1631" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1631" s="10" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B1631" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1631" s="6" t="s">
-        <v>14</v>
+        <v>114</v>
+      </c>
+      <c r="C1631" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1631" s="8" t="s">
         <v>8</v>
@@ -33444,10 +33466,10 @@
     </row>
     <row r="1632" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1632" s="10" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B1632" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C1632" s="5" t="s">
         <v>11</v>
@@ -33458,10 +33480,10 @@
     </row>
     <row r="1633" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1633" s="10" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B1633" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C1633" s="4" t="s">
         <v>7</v>
@@ -33472,10 +33494,10 @@
     </row>
     <row r="1634" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1634" s="10" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B1634" s="1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C1634" s="5" t="s">
         <v>11</v>
@@ -33486,10 +33508,10 @@
     </row>
     <row r="1635" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1635" s="10" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B1635" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C1635" s="6" t="s">
         <v>14</v>
@@ -33500,10 +33522,10 @@
     </row>
     <row r="1636" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1636" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B1636" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C1636" s="5" t="s">
         <v>11</v>
@@ -33514,13 +33536,13 @@
     </row>
     <row r="1637" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1637" s="10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B1637" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1637" s="5" t="s">
-        <v>11</v>
+        <v>102</v>
+      </c>
+      <c r="C1637" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1637" s="8" t="s">
         <v>8</v>
@@ -33528,10 +33550,10 @@
     </row>
     <row r="1638" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1638" s="10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B1638" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C1638" s="5" t="s">
         <v>11</v>
@@ -33542,13 +33564,13 @@
     </row>
     <row r="1639" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1639" s="10" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B1639" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1639" s="5" t="s">
-        <v>11</v>
+        <v>98</v>
+      </c>
+      <c r="C1639" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1639" s="8" t="s">
         <v>8</v>
@@ -33556,13 +33578,13 @@
     </row>
     <row r="1640" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1640" s="10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B1640" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1640" s="6" t="s">
-        <v>14</v>
+        <v>96</v>
+      </c>
+      <c r="C1640" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1640" s="8" t="s">
         <v>8</v>
@@ -33570,10 +33592,10 @@
     </row>
     <row r="1641" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1641" s="10" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B1641" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C1641" s="5" t="s">
         <v>11</v>
@@ -33584,10 +33606,10 @@
     </row>
     <row r="1642" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1642" s="10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B1642" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C1642" s="5" t="s">
         <v>11</v>
@@ -33598,13 +33620,13 @@
     </row>
     <row r="1643" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1643" s="10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B1643" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1643" s="4" t="s">
-        <v>7</v>
+        <v>90</v>
+      </c>
+      <c r="C1643" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1643" s="8" t="s">
         <v>8</v>
@@ -33612,13 +33634,13 @@
     </row>
     <row r="1644" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1644" s="10" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B1644" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1644" s="4" t="s">
-        <v>7</v>
+        <v>88</v>
+      </c>
+      <c r="C1644" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1644" s="8" t="s">
         <v>8</v>
@@ -33626,13 +33648,13 @@
     </row>
     <row r="1645" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1645" s="10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B1645" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1645" s="6" t="s">
-        <v>14</v>
+        <v>86</v>
+      </c>
+      <c r="C1645" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1645" s="8" t="s">
         <v>8</v>
@@ -33640,10 +33662,10 @@
     </row>
     <row r="1646" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1646" s="10" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B1646" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C1646" s="5" t="s">
         <v>11</v>
@@ -33654,13 +33676,13 @@
     </row>
     <row r="1647" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1647" s="10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B1647" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1647" s="5" t="s">
-        <v>11</v>
+        <v>82</v>
+      </c>
+      <c r="C1647" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1647" s="8" t="s">
         <v>8</v>
@@ -33668,10 +33690,10 @@
     </row>
     <row r="1648" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1648" s="10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B1648" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C1648" s="4" t="s">
         <v>7</v>
@@ -33682,13 +33704,13 @@
     </row>
     <row r="1649" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1649" s="10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B1649" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1649" s="5" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="C1649" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1649" s="8" t="s">
         <v>8</v>
@@ -33696,13 +33718,13 @@
     </row>
     <row r="1650" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1650" s="10" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B1650" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1650" s="6" t="s">
-        <v>14</v>
+        <v>76</v>
+      </c>
+      <c r="C1650" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1650" s="8" t="s">
         <v>8</v>
@@ -33710,10 +33732,10 @@
     </row>
     <row r="1651" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1651" s="10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B1651" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C1651" s="5" t="s">
         <v>11</v>
@@ -33724,13 +33746,13 @@
     </row>
     <row r="1652" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1652" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B1652" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1652" s="5" t="s">
-        <v>11</v>
+        <v>72</v>
+      </c>
+      <c r="C1652" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1652" s="8" t="s">
         <v>8</v>
@@ -33738,13 +33760,13 @@
     </row>
     <row r="1653" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1653" s="10" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B1653" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1653" s="4" t="s">
-        <v>7</v>
+        <v>70</v>
+      </c>
+      <c r="C1653" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1653" s="8" t="s">
         <v>8</v>
@@ -33752,13 +33774,13 @@
     </row>
     <row r="1654" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1654" s="10" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B1654" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1654" s="5" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="C1654" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1654" s="8" t="s">
         <v>8</v>
@@ -33766,13 +33788,13 @@
     </row>
     <row r="1655" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1655" s="10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B1655" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1655" s="6" t="s">
-        <v>14</v>
+        <v>66</v>
+      </c>
+      <c r="C1655" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1655" s="8" t="s">
         <v>8</v>
@@ -33780,10 +33802,10 @@
     </row>
     <row r="1656" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1656" s="10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B1656" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C1656" s="5" t="s">
         <v>11</v>
@@ -33794,13 +33816,13 @@
     </row>
     <row r="1657" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1657" s="10" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B1657" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1657" s="5" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="C1657" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1657" s="8" t="s">
         <v>8</v>
@@ -33808,13 +33830,13 @@
     </row>
     <row r="1658" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1658" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B1658" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1658" s="4" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="C1658" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1658" s="8" t="s">
         <v>8</v>
@@ -33822,52 +33844,52 @@
     </row>
     <row r="1659" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1659" s="10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B1659" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C1659" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1659" s="9" t="b">
-        <v>1</v>
+      <c r="E1659" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1660" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1660" s="10" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B1660" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C1660" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1660" s="9" t="b">
-        <v>1</v>
+      <c r="E1660" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1661" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1661" s="10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B1661" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C1661" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1661" s="9" t="b">
-        <v>1</v>
+      <c r="E1661" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1662" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1662" s="10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B1662" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C1662" s="4" t="s">
         <v>7</v>
@@ -33878,27 +33900,27 @@
     </row>
     <row r="1663" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1663" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B1663" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1663" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1663" s="8" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="C1663" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1663" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1664" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1664" s="10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B1664" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1664" s="6" t="s">
-        <v>14</v>
+        <v>48</v>
+      </c>
+      <c r="C1664" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1664" s="9" t="b">
         <v>1</v>
@@ -33906,10 +33928,10 @@
     </row>
     <row r="1665" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1665" s="10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B1665" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C1665" s="5" t="s">
         <v>11</v>
@@ -33920,13 +33942,13 @@
     </row>
     <row r="1666" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1666" s="10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B1666" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1666" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="C1666" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E1666" s="8" t="s">
         <v>8</v>
@@ -33934,13 +33956,13 @@
     </row>
     <row r="1667" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1667" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B1667" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1667" s="4" t="s">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="C1667" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E1667" s="8" t="s">
         <v>8</v>
@@ -33948,38 +33970,38 @@
     </row>
     <row r="1668" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1668" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B1668" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C1668" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1668" s="8" t="s">
-        <v>8</v>
+      <c r="E1668" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1669" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1669" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B1669" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C1669" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1669" s="8" t="s">
-        <v>8</v>
+      <c r="E1669" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1670" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1670" s="10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B1670" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C1670" s="5" t="s">
         <v>11</v>
@@ -33990,10 +34012,10 @@
     </row>
     <row r="1671" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1671" s="10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B1671" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C1671" s="4" t="s">
         <v>7</v>
@@ -34004,13 +34026,13 @@
     </row>
     <row r="1672" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1672" s="10" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B1672" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1672" s="5" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="C1672" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E1672" s="8" t="s">
         <v>8</v>
@@ -34018,38 +34040,38 @@
     </row>
     <row r="1673" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1673" s="10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B1673" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1673" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1673" s="9" t="b">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C1673" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1673" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1674" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1674" s="10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1674" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C1674" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1674" s="9" t="b">
-        <v>1</v>
+      <c r="E1674" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1675" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1675" s="10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B1675" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C1675" s="4" t="s">
         <v>7</v>
@@ -34060,10 +34082,10 @@
     </row>
     <row r="1676" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1676" s="10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1676" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C1676" s="5" t="s">
         <v>11</v>
@@ -34074,149 +34096,206 @@
     </row>
     <row r="1677" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1677" s="10" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B1677" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C1677" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1677" s="8" t="s">
-        <v>8</v>
+      <c r="E1677" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1678" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1678" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B1678" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C1678" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1678" s="8" t="s">
-        <v>8</v>
+      <c r="E1678" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1679" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1679" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1679" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1679" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1679" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1680" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1680" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1680" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1680" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1681" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1681" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1681" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1681" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1682" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1682" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1682" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1682" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1683" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1679" s="1" t="s">
+      <c r="B1683" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1679" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1679" s="8" t="s">
+      <c r="C1683" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1683" s="8" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1679">
-    <sortCondition ref="A2:A1679"/>
+  <autoFilter ref="E1:E1683" xr:uid="{29D7626E-60CB-4C18-9B7D-C0EAF0F7B115}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1681">
+    <sortCondition ref="A2:A1681"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B1679" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B1678" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B1677" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B1676" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B1675" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B1674" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B1673" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B1672" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B1671" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B1670" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B1669" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B1668" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B1667" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B1666" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B1665" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B1664" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B1663" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B1662" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B1661" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B1660" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B1659" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B1658" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B1657" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B1656" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B1655" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B1654" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B1653" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B1652" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B1651" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B1650" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B1649" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B1648" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B1647" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B1646" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B1645" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B1644" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B1643" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B1642" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B1641" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B1640" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B1639" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B1638" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B1637" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B1636" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B1635" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B1634" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B1633" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B1632" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B1631" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B1630" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B1629" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B1628" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B1627" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B1626" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B1625" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B1624" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B1623" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B1622" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B1621" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B1620" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B1619" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B1618" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B1617" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B1616" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B1615" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B1614" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B1613" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B1612" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B1611" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B1610" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B1609" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B1608" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B1607" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B1606" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B1605" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B1604" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B1603" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B1602" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B1601" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B1600" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B1599" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B1598" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B1597" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B1596" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B1595" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B1594" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B1593" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B1592" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B1591" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B1590" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B1589" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B1588" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B1587" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B1586" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B1585" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B1584" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B1583" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B1582" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B1683" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B1682" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B1681" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B1680" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B1679" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B1678" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B1677" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B1676" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B1675" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B1674" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B1673" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B1672" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B1671" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B1670" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B1669" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B1668" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B1667" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B1666" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B1665" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B1664" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B1663" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B1662" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B1661" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B1660" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B1659" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B1658" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B1657" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B1656" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B1655" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B1654" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B1653" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B1652" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B1651" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B1650" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B1649" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B1648" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B1647" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B1646" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B1645" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B1644" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B1643" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B1642" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B1641" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B1640" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B1639" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B1638" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B1637" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B1636" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B1635" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B1634" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B1633" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B1632" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B1631" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B1630" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B1629" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B1628" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B1627" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B1626" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B1625" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B1624" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B1623" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B1622" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B1621" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B1620" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B1619" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B1618" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B1617" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B1616" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B1615" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B1614" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B1613" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B1612" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B1611" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B1610" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B1609" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B1608" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B1607" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B1606" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B1605" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B1604" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B1603" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B1602" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B1601" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B1600" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B1599" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B1598" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B1597" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B1596" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B1595" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B1594" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B1593" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B1592" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B1591" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B1590" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B1589" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B1588" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B1587" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B1586" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
     <hyperlink ref="B1581" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
     <hyperlink ref="B1580" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
     <hyperlink ref="B1579" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
@@ -35800,8 +35879,12 @@
     <hyperlink ref="D32" r:id="rId1679" xr:uid="{6783BC4D-2322-4ECC-B313-3BFDFD03DD43}"/>
     <hyperlink ref="D601" r:id="rId1680" xr:uid="{2DCDBBE1-8A88-4973-888C-44C13ECC1C30}"/>
     <hyperlink ref="D110" r:id="rId1681" xr:uid="{7951F06E-2736-42EC-A89A-9BDAE04BE39E}"/>
+    <hyperlink ref="B1582" r:id="rId1682" display="Maximum Number of Events That Can Be Attended II" xr:uid="{56F71FD5-ADE5-4CC9-A769-1F8B0D1730C9}"/>
+    <hyperlink ref="B1583" r:id="rId1683" xr:uid="{5BD426F5-E583-4EE7-AB2A-D48D76226D00}"/>
+    <hyperlink ref="B1584" r:id="rId1684" xr:uid="{E5518524-D9F1-4C4B-935C-470E866CB3FC}"/>
+    <hyperlink ref="B1585" r:id="rId1685" display="Maximum Distance Between a Pair of Values" xr:uid="{584CCACC-14CC-4279-B0FC-FB5CCD150E0F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1682"/>
+  <pageSetup orientation="portrait" r:id="rId1686"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved Hard problem with Binary Search
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B15A64-E7DA-4A48-B8D1-612B4360C1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C12AD7-B2AC-45AB-ACC2-59BA74ADEE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6618" uniqueCount="3379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6617" uniqueCount="3379">
   <si>
     <t>ID</t>
   </si>
@@ -10591,8 +10591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1580" workbookViewId="0">
-      <selection activeCell="J1580" sqref="J1580"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="E394" sqref="E394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16130,8 +16130,8 @@
       <c r="C394" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E394" s="8" t="s">
-        <v>8</v>
+      <c r="E394" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="395" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Daily Challenge Problem
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C12AD7-B2AC-45AB-ACC2-59BA74ADEE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F1B17-5F9D-46F1-B2F3-772479659B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6617" uniqueCount="3379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6617" uniqueCount="3380">
   <si>
     <t>ID</t>
   </si>
@@ -10168,6 +10168,9 @@
   </si>
   <si>
     <t>Maximum Subarray Min-Product</t>
+  </si>
+  <si>
+    <t>Prefix Sum and Fixed Sliding Window</t>
   </si>
 </sst>
 </file>
@@ -10591,8 +10594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="E394" sqref="E394"/>
+    <sheetView tabSelected="1" topLeftCell="A1316" workbookViewId="0">
+      <selection activeCell="D1328" sqref="D1328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -29218,8 +29221,11 @@
       <c r="C1328" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1328" s="8" t="s">
-        <v>8</v>
+      <c r="D1328" t="s">
+        <v>3379</v>
+      </c>
+      <c r="E1328" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1329" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 1482. Minimum Number of Days to Make m Bouquets
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F1B17-5F9D-46F1-B2F3-772479659B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424AE008-7717-4503-81CA-41C4E0AD1B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6617" uniqueCount="3380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6617" uniqueCount="3381">
   <si>
     <t>ID</t>
   </si>
@@ -10171,6 +10171,9 @@
   </si>
   <si>
     <t>Prefix Sum and Fixed Sliding Window</t>
+  </si>
+  <si>
+    <t>Explanation in Solution File, Binary Search</t>
   </si>
 </sst>
 </file>
@@ -10594,8 +10597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1316" workbookViewId="0">
-      <selection activeCell="D1328" sqref="D1328"/>
+    <sheetView tabSelected="1" topLeftCell="A1360" workbookViewId="0">
+      <selection activeCell="G1366" sqref="G1366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -29840,8 +29843,11 @@
       <c r="C1372" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1372" s="8" t="s">
-        <v>8</v>
+      <c r="D1372" t="s">
+        <v>3380</v>
+      </c>
+      <c r="E1372" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1373" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Leetcode dailly problem after hint, was quite tricky due to edge cases
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROHAN\Desktop\CP-Prac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985D5106-6DD8-4CDA-86C7-AF05A9C008AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCB415-2A50-4C61-81C5-2A0F36A52928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6670" uniqueCount="3402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6670" uniqueCount="3403">
   <si>
     <t>ID</t>
   </si>
@@ -10237,6 +10237,9 @@
   </si>
   <si>
     <t>Check if Word Equals Summation of Two Words</t>
+  </si>
+  <si>
+    <t>https://bit.ly/3h9YkTw</t>
   </si>
 </sst>
 </file>
@@ -10666,8 +10669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
+      <selection activeCell="G594" sqref="G594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19005,8 +19008,11 @@
       <c r="C594" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E594" s="8" t="s">
-        <v>8</v>
+      <c r="D594" s="1" t="s">
+        <v>3402</v>
+      </c>
+      <c r="E594" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="595" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 	 Number of Sub-arrays of Size K and Average Greater than or Equal to Threshold
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D73686A-A8C5-42EB-A2AA-74CE1486E05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA36463-214C-4D2D-94EB-D74226C7D408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6671" uniqueCount="3403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6670" uniqueCount="3403">
   <si>
     <t>ID</t>
   </si>
@@ -10669,8 +10669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" workbookViewId="0">
-      <selection activeCell="A1701" sqref="A1701"/>
+    <sheetView tabSelected="1" topLeftCell="A1239" workbookViewId="0">
+      <selection activeCell="E1250" sqref="E1250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28207,8 +28207,8 @@
       <c r="C1250" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1250" s="8" t="s">
-        <v>8</v>
+      <c r="E1250" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1251" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 2 Tree questions
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA36463-214C-4D2D-94EB-D74226C7D408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAD5A7D-3673-410F-9683-3226AC8F27F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6670" uniqueCount="3403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6669" uniqueCount="3404">
   <si>
     <t>ID</t>
   </si>
@@ -10240,6 +10240,9 @@
   </si>
   <si>
     <t>https://bit.ly/3h9YkTw</t>
+  </si>
+  <si>
+    <t>IMPORTANT CONCEPT</t>
   </si>
 </sst>
 </file>
@@ -10669,8 +10672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1239" workbookViewId="0">
-      <selection activeCell="E1250" sqref="E1250"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12103,8 +12106,8 @@
       <c r="C101" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="8" t="s">
-        <v>8</v>
+      <c r="E101" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -12117,8 +12120,11 @@
       <c r="C102" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E102" s="8" t="s">
-        <v>8</v>
+      <c r="D102" t="s">
+        <v>3403</v>
+      </c>
+      <c r="E102" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
solved Kth smallest element in BST
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAD5A7D-3673-410F-9683-3226AC8F27F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E14739C-9EE6-4B9C-BFF9-A1F6D8568EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10672,8 +10672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12106,6 +12106,9 @@
       <c r="C101" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="D101" t="s">
+        <v>3403</v>
+      </c>
       <c r="E101" s="9" t="b">
         <v>1</v>
       </c>
@@ -13708,8 +13711,8 @@
       <c r="C215" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E215" s="8" t="s">
-        <v>8</v>
+      <c r="E215" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Max Area of Island
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893B61B-9E16-4748-97D0-C182B9CFCF68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69E162E-6D80-47C5-9138-0B5581D76527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6668" uniqueCount="3404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6667" uniqueCount="3404">
   <si>
     <t>ID</t>
   </si>
@@ -10672,8 +10672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A724" workbookViewId="0">
-      <selection activeCell="D738" sqref="D738"/>
+    <sheetView tabSelected="1" topLeftCell="A620" workbookViewId="0">
+      <selection activeCell="E631" sqref="E631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19541,8 +19541,8 @@
       <c r="C631" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E631" s="8" t="s">
-        <v>8</v>
+      <c r="E631" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="632" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Video stitching greedily, explanation added in code
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F6BB30-B6C1-475B-B0B7-78E5F672139F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253426C0-C8D2-45BB-911C-DE9DB08C9328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,19 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$E$1:$E$1687</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="3404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="3405">
   <si>
     <t>ID</t>
   </si>
@@ -10243,6 +10235,9 @@
   </si>
   <si>
     <t>IMPORTANT CONCEPT</t>
+  </si>
+  <si>
+    <t>REVISE GREEDY EXPLANATION</t>
   </si>
 </sst>
 </file>
@@ -10672,8 +10667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="B441" sqref="B441"/>
+    <sheetView tabSelected="1" topLeftCell="A992" workbookViewId="0">
+      <selection activeCell="D999" sqref="D999"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -24632,8 +24627,11 @@
       <c r="C994" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E994" s="8" t="s">
-        <v>8</v>
+      <c r="D994" t="s">
+        <v>3404</v>
+      </c>
+      <c r="E994" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="995" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Path Sum II
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253426C0-C8D2-45BB-911C-DE9DB08C9328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBBE7EE-B6C5-4DF2-803C-FE9B019E6A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="3405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6665" uniqueCount="3405">
   <si>
     <t>ID</t>
   </si>
@@ -10667,8 +10667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A992" workbookViewId="0">
-      <selection activeCell="D999" sqref="D999"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12292,8 +12292,8 @@
       <c r="C114" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E114" s="8" t="s">
-        <v>8</v>
+      <c r="E114" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Explanation of Two City Scheduling added
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A9307F-A0CA-47C2-91EC-ECE1416F0C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE98D4-1DF5-4CBF-8DA0-110C934144E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="3405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="3406">
   <si>
     <t>ID</t>
   </si>
@@ -10238,6 +10238,9 @@
   </si>
   <si>
     <t>REVISE GREEDY EXPLANATION</t>
+  </si>
+  <si>
+    <t>Explanation in Java file itself</t>
   </si>
 </sst>
 </file>
@@ -10667,8 +10670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
+      <selection activeCell="D1008" sqref="D1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -24829,8 +24832,11 @@
       <c r="C1008" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1008" s="8" t="s">
-        <v>8</v>
+      <c r="D1008" t="s">
+        <v>3405</v>
+      </c>
+      <c r="E1008" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1009" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Minimum Number of Arrows to Burst Balloons
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE98D4-1DF5-4CBF-8DA0-110C934144E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01680E97-63BB-497E-8E6E-848E3DF7BD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="3406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="3407">
   <si>
     <t>ID</t>
   </si>
@@ -10241,6 +10241,9 @@
   </si>
   <si>
     <t>Explanation in Java file itself</t>
+  </si>
+  <si>
+    <t>Greedy, Done in one go</t>
   </si>
 </sst>
 </file>
@@ -10670,8 +10673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
-      <selection activeCell="D1008" sqref="D1008"/>
+    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="D429" sqref="D429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16722,8 +16725,11 @@
       <c r="C430" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E430" s="8" t="s">
-        <v>8</v>
+      <c r="D430" t="s">
+        <v>3406</v>
+      </c>
+      <c r="E430" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Remove Nth node from End of LInked List
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116A49D-368F-4EF8-97DE-1B9E27753B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF46F9-8E46-4C42-AE46-D4811181E25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6661" uniqueCount="3410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3410">
   <si>
     <t>ID</t>
   </si>
@@ -10682,8 +10682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
-      <selection activeCell="D414" sqref="D414"/>
+    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
+      <selection activeCell="D464" sqref="D464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10973,8 +10973,8 @@
       <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>8</v>
+      <c r="E20" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Hard Problem : Maximum Profit in Job Scheduling (DP + Binary Search)
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF46F9-8E46-4C42-AE46-D4811181E25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1FECB8-9D22-4F6F-B7D5-DEF0481AD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3411">
   <si>
     <t>ID</t>
   </si>
@@ -10253,6 +10253,9 @@
   </si>
   <si>
     <t>Explanation in py file itself</t>
+  </si>
+  <si>
+    <t>Reference Links in Java File</t>
   </si>
 </sst>
 </file>
@@ -10682,8 +10685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
-      <selection activeCell="D464" sqref="D464"/>
+    <sheetView tabSelected="1" topLeftCell="A1297" workbookViewId="0">
+      <selection activeCell="D1310" sqref="D1310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27435,8 +27438,11 @@
       <c r="C1192" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1192" s="8" t="s">
-        <v>8</v>
+      <c r="D1192" t="s">
+        <v>3410</v>
+      </c>
+      <c r="E1192" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1193" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a BFS problem
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C310D7-5480-440E-9DAE-878EA075D77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768B52D-A190-4853-A064-1811941B94D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3413">
   <si>
     <t>ID</t>
   </si>
@@ -10256,6 +10256,12 @@
   </si>
   <si>
     <t>Reference Links in Java File</t>
+  </si>
+  <si>
+    <t>Nearest Exit from Entrance in Maze</t>
+  </si>
+  <si>
+    <t>BFS</t>
   </si>
 </sst>
 </file>
@@ -10685,8 +10691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A1677" workbookViewId="0">
+      <selection activeCell="I1681" sqref="I1681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34515,13 +34521,16 @@
         <v>184</v>
       </c>
       <c r="B1697" s="1" t="s">
-        <v>3400</v>
+        <v>3411</v>
       </c>
       <c r="C1697" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1697" s="8" t="s">
-        <v>8</v>
+      <c r="D1697" t="s">
+        <v>3412</v>
+      </c>
+      <c r="E1697" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1698" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -36263,7 +36272,7 @@
     <hyperlink ref="B1695" r:id="rId1697" xr:uid="{37961FD1-71CB-4461-A522-3021DB033097}"/>
     <hyperlink ref="B1692" r:id="rId1698" display="Sum of Floored Pairs" xr:uid="{14D8402C-75A7-4E49-A56A-C48646E943CF}"/>
     <hyperlink ref="B1696" r:id="rId1699" xr:uid="{8CC21C31-E2DD-4D84-B695-0BF6FC723057}"/>
-    <hyperlink ref="B1697" r:id="rId1700" xr:uid="{E7065A0C-0538-41CF-9F36-A65E05173C49}"/>
+    <hyperlink ref="B1697" r:id="rId1700" display="Stone Game VIII" xr:uid="{E7065A0C-0538-41CF-9F36-A65E05173C49}"/>
     <hyperlink ref="B1698" r:id="rId1701" xr:uid="{D320B814-2D4C-496A-98F7-5CB452A4AB48}"/>
     <hyperlink ref="B1699" r:id="rId1702" xr:uid="{BE3FFEBE-4FD0-4D58-8E59-155F1AB41174}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Solved Delete and Earn , Nim Game, Course Schedule 2
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768B52D-A190-4853-A064-1811941B94D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94540E9-7284-4231-BF08-245A16358F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6660" uniqueCount="3413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6659" uniqueCount="3414">
   <si>
     <t>ID</t>
   </si>
@@ -10262,6 +10262,9 @@
   </si>
   <si>
     <t>BFS</t>
+  </si>
+  <si>
+    <t>DP, Explanation in code file</t>
   </si>
 </sst>
 </file>
@@ -10691,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1677" workbookViewId="0">
-      <selection activeCell="I1681" sqref="I1681"/>
+    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="A665" sqref="A665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14590,8 +14593,8 @@
       <c r="C276" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E276" s="8" t="s">
-        <v>8</v>
+      <c r="E276" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -20054,8 +20057,11 @@
       <c r="C665" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E665" s="8" t="s">
-        <v>8</v>
+      <c r="D665" t="s">
+        <v>3413</v>
+      </c>
+      <c r="E665" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="666" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Unique Paths Solved in One go
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CF39FD-CFED-4880-8730-460B35159C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782CA3E3-A4C0-49B9-9721-EE4116DE48D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6658" uniqueCount="3414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6657" uniqueCount="3414">
   <si>
     <t>ID</t>
   </si>
@@ -10694,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A993" workbookViewId="0">
-      <selection activeCell="D1006" sqref="D1006"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11599,8 +11599,8 @@
       <c r="C63" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="8" t="s">
-        <v>8</v>
+      <c r="E63" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Binary Tree Pruning
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782CA3E3-A4C0-49B9-9721-EE4116DE48D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDC0B1F-4667-4ADD-8980-BA404C2E94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10694,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
+      <selection activeCell="E757" sqref="E757"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -21348,8 +21348,11 @@
       <c r="C757" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E757" s="8" t="s">
-        <v>8</v>
+      <c r="D757" t="s">
+        <v>3405</v>
+      </c>
+      <c r="E757" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="758" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved problem based on Edit DIstance concept
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDC0B1F-4667-4ADD-8980-BA404C2E94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40650CC-6964-4C0B-A472-2BCB446272BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6657" uniqueCount="3414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6656" uniqueCount="3414">
   <si>
     <t>ID</t>
   </si>
@@ -10694,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
-      <selection activeCell="E757" sqref="E757"/>
+    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
+      <selection activeCell="D634" activeCellId="1" sqref="G636 D634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19665,8 +19665,8 @@
       <c r="C637" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E637" s="8" t="s">
-        <v>8</v>
+      <c r="E637" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="638" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Matrix Block Sum using 2D prefix sum
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40650CC-6964-4C0B-A472-2BCB446272BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6E2499-4EE3-42CD-82D4-BED84118D0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6656" uniqueCount="3414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6653" uniqueCount="3414">
   <si>
     <t>ID</t>
   </si>
@@ -10694,8 +10694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="D634" activeCellId="1" sqref="G636 D634"/>
+    <sheetView tabSelected="1" topLeftCell="A1111" workbookViewId="0">
+      <selection activeCell="E1123" sqref="E1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10943,8 +10943,8 @@
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>8</v>
+      <c r="E17" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -17920,8 +17920,8 @@
       <c r="C513" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E513" s="8" t="s">
-        <v>8</v>
+      <c r="E513" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="514" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -26493,8 +26493,8 @@
       <c r="C1123" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1123" s="8" t="s">
-        <v>8</v>
+      <c r="E1123" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1124" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Minimum Limit of Balls in a Bag --- Tricky problem
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A9973B-D030-48B3-B13D-42583941FB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D120EAA5-3B2B-4D7F-982D-03911DE32EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3415">
   <si>
     <t>ID</t>
   </si>
@@ -10265,6 +10265,9 @@
   </si>
   <si>
     <t>DP, Explanation in code file</t>
+  </si>
+  <si>
+    <t>https://youtu.be/znZ4wT1L8Y0</t>
   </si>
 </sst>
 </file>
@@ -10694,8 +10697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1546" workbookViewId="0">
-      <selection activeCell="E1560" sqref="E1560"/>
+    <sheetView tabSelected="1" topLeftCell="A1585" workbookViewId="0">
+      <selection activeCell="D1594" sqref="D1594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33250,8 +33253,11 @@
       <c r="C1605" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1605" s="8" t="s">
-        <v>8</v>
+      <c r="D1605" s="1" t="s">
+        <v>3414</v>
+      </c>
+      <c r="E1605" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1606" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -36287,8 +36293,9 @@
     <hyperlink ref="B1697" r:id="rId1700" display="Stone Game VIII" xr:uid="{E7065A0C-0538-41CF-9F36-A65E05173C49}"/>
     <hyperlink ref="B1698" r:id="rId1701" xr:uid="{D320B814-2D4C-496A-98F7-5CB452A4AB48}"/>
     <hyperlink ref="B1699" r:id="rId1702" xr:uid="{BE3FFEBE-4FD0-4D58-8E59-155F1AB41174}"/>
+    <hyperlink ref="D1605" r:id="rId1703" xr:uid="{0D40AF47-4380-4A3C-B92C-6961B6E391DF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1703"/>
+  <pageSetup orientation="portrait" r:id="rId1704"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved Some math and KMP questions
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D120EAA5-3B2B-4D7F-982D-03911DE32EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5834A73D-E624-470A-990E-351A8526ABD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3417">
   <si>
     <t>ID</t>
   </si>
@@ -10268,6 +10268,25 @@
   </si>
   <si>
     <t>https://youtu.be/znZ4wT1L8Y0</t>
+  </si>
+  <si>
+    <t>KMP Algo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Similar to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Minimum Appends to make Palindrome</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -10697,16 +10716,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1585" workbookViewId="0">
-      <selection activeCell="D1594" sqref="D1594"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="58.6640625" customWidth="1"/>
     <col min="3" max="3" width="25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -13518,8 +13537,11 @@
       <c r="C199" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E199" s="8" t="s">
-        <v>8</v>
+      <c r="D199" t="s">
+        <v>3416</v>
+      </c>
+      <c r="E199" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -29019,8 +29041,11 @@
       <c r="C1303" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1303" s="8" t="s">
-        <v>8</v>
+      <c r="D1303" t="s">
+        <v>3415</v>
+      </c>
+      <c r="E1303" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1304" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Minimum Path Sum
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FA128F-4BCB-48FA-82EB-0F453950F745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E26F3B-3A57-44DF-A667-4E2D1154DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3418">
   <si>
     <t>ID</t>
   </si>
@@ -10287,6 +10287,9 @@
       </rPr>
       <t>Minimum Appends to make Palindrome</t>
     </r>
+  </si>
+  <si>
+    <t>Simple DP</t>
   </si>
 </sst>
 </file>
@@ -10716,8 +10719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A816" workbookViewId="0">
-      <selection activeCell="E827" sqref="E827"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11649,8 +11652,11 @@
       <c r="C65" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E65" s="8" t="s">
-        <v>8</v>
+      <c r="D65" t="s">
+        <v>3417</v>
+      </c>
+      <c r="E65" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Jump Game III
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E26F3B-3A57-44DF-A667-4E2D1154DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C92E109-4655-4429-BBA8-894FE3E35049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3419">
   <si>
     <t>ID</t>
   </si>
@@ -10290,6 +10290,9 @@
   </si>
   <si>
     <t>Simple DP</t>
+  </si>
+  <si>
+    <t>BFS on array</t>
   </si>
 </sst>
 </file>
@@ -10719,8 +10722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A1233" workbookViewId="0">
+      <selection activeCell="D1239" sqref="D1239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28137,8 +28140,11 @@
       <c r="C1238" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1238" s="8" t="s">
-        <v>8</v>
+      <c r="D1238" t="s">
+        <v>3418</v>
+      </c>
+      <c r="E1238" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1239" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Critical Connections in a Network
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882CC44-0B5B-4B36-A807-7ED0E102FD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B5B5A9-23F5-4D18-9728-4121A7DECFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3420">
   <si>
     <t>ID</t>
   </si>
@@ -10293,6 +10293,9 @@
   </si>
   <si>
     <t>BFS on array</t>
+  </si>
+  <si>
+    <t>Finding Bridges in a Graph</t>
   </si>
 </sst>
 </file>
@@ -10722,8 +10725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A1156" workbookViewId="0">
+      <selection activeCell="D1168" sqref="D1168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27143,8 +27146,11 @@
       <c r="C1167" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1167" s="8" t="s">
-        <v>8</v>
+      <c r="D1167" t="s">
+        <v>3419</v>
+      </c>
+      <c r="E1167" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1168" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Minimum Height Trees
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B5B5A9-23F5-4D18-9728-4121A7DECFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F604DECD-131A-4B60-AC12-1372E1D4DF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3421">
   <si>
     <t>ID</t>
   </si>
@@ -10296,6 +10296,9 @@
   </si>
   <si>
     <t>Finding Bridges in a Graph</t>
+  </si>
+  <si>
+    <t>Finding Tree Center(s)</t>
   </si>
 </sst>
 </file>
@@ -10725,8 +10728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1156" workbookViewId="0">
-      <selection activeCell="D1168" sqref="D1168"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="D294" sqref="D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14882,8 +14885,11 @@
       <c r="C294" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E294" s="8" t="s">
-        <v>8</v>
+      <c r="D294" t="s">
+        <v>3420</v>
+      </c>
+      <c r="E294" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved lots of question on trees
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F604DECD-131A-4B60-AC12-1372E1D4DF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF125140-32A9-4B84-87D4-BED055229726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3422">
   <si>
     <t>ID</t>
   </si>
@@ -10299,6 +10299,9 @@
   </si>
   <si>
     <t>Finding Tree Center(s)</t>
+  </si>
+  <si>
+    <t>Binary Lifting</t>
   </si>
 </sst>
 </file>
@@ -10728,8 +10731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="D294" sqref="D294"/>
+    <sheetView tabSelected="1" topLeftCell="A1137" workbookViewId="0">
+      <selection activeCell="G1162" sqref="G1162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27096,8 +27099,11 @@
       <c r="C1163" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1163" s="8" t="s">
-        <v>8</v>
+      <c r="D1163" t="s">
+        <v>3421</v>
+      </c>
+      <c r="E1163" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1164" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a trie question on LC
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF125140-32A9-4B84-87D4-BED055229726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3900207A-015B-41E5-A816-C18DFD0F7B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3423">
   <si>
     <t>ID</t>
   </si>
@@ -10302,6 +10302,9 @@
   </si>
   <si>
     <t>Binary Lifting</t>
+  </si>
+  <si>
+    <t>Usage of Trie</t>
   </si>
 </sst>
 </file>
@@ -10731,8 +10734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1137" workbookViewId="0">
-      <selection activeCell="G1162" sqref="G1162"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13513,8 +13516,11 @@
       <c r="C196" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E196" s="8" t="s">
-        <v>8</v>
+      <c r="D196" t="s">
+        <v>3422</v>
+      </c>
+      <c r="E196" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved lots of problems
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3900207A-015B-41E5-A816-C18DFD0F7B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB908E1-4568-48C7-BDF5-58F005DF6D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3428">
   <si>
     <t>ID</t>
   </si>
@@ -10305,6 +10305,21 @@
   </si>
   <si>
     <t>Usage of Trie</t>
+  </si>
+  <si>
+    <t>Last Day Where You Can Still Cross</t>
+  </si>
+  <si>
+    <t>Binary Search + BFS</t>
+  </si>
+  <si>
+    <t>Array With Elements Not Equal to Average of Neighbors</t>
+  </si>
+  <si>
+    <t>1877</t>
+  </si>
+  <si>
+    <t>Explanation in Python File</t>
   </si>
 </sst>
 </file>
@@ -10734,8 +10749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="D195" sqref="D195"/>
+    <sheetView tabSelected="1" topLeftCell="A1686" workbookViewId="0">
+      <selection activeCell="F1697" sqref="F1697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34617,13 +34632,16 @@
         <v>182</v>
       </c>
       <c r="B1698" s="1" t="s">
-        <v>3400</v>
+        <v>3425</v>
       </c>
       <c r="C1698" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1698" s="8" t="s">
-        <v>8</v>
+      <c r="D1698" t="s">
+        <v>3427</v>
+      </c>
+      <c r="E1698" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1699" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -34631,18 +34649,21 @@
         <v>180</v>
       </c>
       <c r="B1699" s="1" t="s">
-        <v>3400</v>
+        <v>3423</v>
       </c>
       <c r="C1699" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1699" s="8" t="s">
-        <v>8</v>
+      <c r="D1699" t="s">
+        <v>3424</v>
+      </c>
+      <c r="E1699" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1700" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1700" s="11" t="s">
-        <v>180</v>
+        <v>3426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved a pronlem on Leetcode
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB908E1-4568-48C7-BDF5-58F005DF6D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03E381B-F415-40C5-B05B-166B534352D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3428">
   <si>
     <t>ID</t>
   </si>
@@ -10749,8 +10749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1686" workbookViewId="0">
-      <selection activeCell="F1697" sqref="F1697"/>
+    <sheetView tabSelected="1" topLeftCell="A1218" workbookViewId="0">
+      <selection activeCell="H1231" sqref="H1231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28011,8 +28011,8 @@
       <c r="C1226" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1226" s="8" t="s">
-        <v>8</v>
+      <c r="E1226" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1227" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a HARD DP problem
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079642C1-4504-4D9E-82FA-7E15553A63B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA606F-4D6F-4B7A-B624-5AA74D62E589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10752,8 +10752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1375" workbookViewId="0">
-      <selection activeCell="D1398" sqref="D1398"/>
+    <sheetView tabSelected="1" topLeftCell="B1171" workbookViewId="0">
+      <selection activeCell="D1183" sqref="D1183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12537,8 +12537,11 @@
       <c r="C125" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E125" s="8" t="s">
-        <v>8</v>
+      <c r="D125" t="s">
+        <v>3428</v>
+      </c>
+      <c r="E125" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -27395,8 +27398,11 @@
       <c r="C1182" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1182" s="8" t="s">
-        <v>8</v>
+      <c r="D1182" t="s">
+        <v>3405</v>
+      </c>
+      <c r="E1182" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1183" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 985. Sum of Even Numbers After Queries
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA606F-4D6F-4B7A-B624-5AA74D62E589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0FEB46-EF7A-43D9-801A-C7AC2F206EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10752,8 +10752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1171" workbookViewId="0">
-      <selection activeCell="D1183" sqref="D1183"/>
+    <sheetView tabSelected="1" topLeftCell="B929" workbookViewId="0">
+      <selection activeCell="D940" sqref="D940"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23986,11 +23986,14 @@
       <c r="B940" s="1" t="s">
         <v>1487</v>
       </c>
-      <c r="C940" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E940" s="8" t="s">
-        <v>8</v>
+      <c r="C940" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D940" t="s">
+        <v>3369</v>
+      </c>
+      <c r="E940" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="941" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Palindromic Subtrings --- DP question
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0FEB46-EF7A-43D9-801A-C7AC2F206EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5372DF86-E71F-4092-B4F4-86730744CE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3430">
   <si>
     <t>ID</t>
   </si>
@@ -10323,6 +10323,9 @@
   </si>
   <si>
     <t>Explanation in code file</t>
+  </si>
+  <si>
+    <t>https://youtu.be/XmSOWnL6T_I</t>
   </si>
 </sst>
 </file>
@@ -10752,8 +10755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B929" workbookViewId="0">
-      <selection activeCell="D940" sqref="D940"/>
+    <sheetView tabSelected="1" topLeftCell="B560" workbookViewId="0">
+      <selection activeCell="D569" sqref="D569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18976,8 +18979,11 @@
       <c r="C583" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E583" s="8" t="s">
-        <v>8</v>
+      <c r="D583" s="1" t="s">
+        <v>3429</v>
+      </c>
+      <c r="E583" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="584" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -36391,8 +36397,9 @@
     <hyperlink ref="B1698" r:id="rId1701" xr:uid="{D320B814-2D4C-496A-98F7-5CB452A4AB48}"/>
     <hyperlink ref="B1699" r:id="rId1702" xr:uid="{BE3FFEBE-4FD0-4D58-8E59-155F1AB41174}"/>
     <hyperlink ref="D1605" r:id="rId1703" xr:uid="{0D40AF47-4380-4A3C-B92C-6961B6E391DF}"/>
+    <hyperlink ref="D583" r:id="rId1704" xr:uid="{61FA88FA-2D4F-4048-BCC5-501F7B008612}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1704"/>
+  <pageSetup orientation="portrait" r:id="rId1705"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved Longest Palindrome Substring
</commit_message>
<xml_diff>
--- a/Leetcode_FULL.xlsx
+++ b/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5372DF86-E71F-4092-B4F4-86730744CE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025B523D-7322-482A-96E2-9ED74B97C7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3431">
   <si>
     <t>ID</t>
   </si>
@@ -10326,6 +10326,9 @@
   </si>
   <si>
     <t>https://youtu.be/XmSOWnL6T_I</t>
+  </si>
+  <si>
+    <t>Very similar to LC : Count Palindromes</t>
   </si>
 </sst>
 </file>
@@ -10755,8 +10758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B560" workbookViewId="0">
-      <selection activeCell="D569" sqref="D569"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10850,8 +10853,11 @@
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>8</v>
+      <c r="D6" t="s">
+        <v>3430</v>
+      </c>
+      <c r="E6" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>